<commit_message>
Common function and input data
</commit_message>
<xml_diff>
--- a/ERP_Hybrid/TestInput/HybridData.xlsx
+++ b/ERP_Hybrid/TestInput/HybridData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinad\git\OJTEveningBatch\ERP_Hybrid\TestInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532332C7-E21B-4C11-A6FC-D23332DA6D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17BD2D2-E815-4A11-808F-B61C984AC7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t xml:space="preserve">TC ID </t>
   </si>
@@ -79,23 +79,122 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Function Name</t>
-  </si>
-  <si>
-    <t>Locator type</t>
-  </si>
-  <si>
-    <t>Locator value</t>
-  </si>
-  <si>
     <t>TestData</t>
+  </si>
+  <si>
+    <t>FunctionName</t>
+  </si>
+  <si>
+    <t>LocatorType</t>
+  </si>
+  <si>
+    <t>Launch browser</t>
+  </si>
+  <si>
+    <t>startBrowser</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Launch url in a browser</t>
+  </si>
+  <si>
+    <t>openApplication</t>
+  </si>
+  <si>
+    <t>wait for username</t>
+  </si>
+  <si>
+    <t>waitForElement</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>typeAction</t>
+  </si>
+  <si>
+    <t>wait for password</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>wait for login button</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>click login</t>
+  </si>
+  <si>
+    <t>clickAction</t>
+  </si>
+  <si>
+    <t>wait for logout</t>
+  </si>
+  <si>
+    <t>verify title</t>
+  </si>
+  <si>
+    <t>validateTitle</t>
+  </si>
+  <si>
+    <t>click logout</t>
+  </si>
+  <si>
+    <t>wait for ok button</t>
+  </si>
+  <si>
+    <t>click ok button</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>LocatorValue</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>btnsubmit</t>
+  </si>
+  <si>
+    <t>//a[@id='logout']</t>
+  </si>
+  <si>
+    <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +202,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,8 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -491,42 +614,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5914AB1-9DF7-4B52-879F-6204673EC0F3}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>